<commit_message>
Aggiornato giacenza.xlsx da lbianco via Streamlit
</commit_message>
<xml_diff>
--- a/giacenza.xlsx
+++ b/giacenza.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Data</t>
   </si>
@@ -30,9 +30,6 @@
     <t>FUCILE FRANCESCO</t>
   </si>
   <si>
-    <t>GANCI CORRADO</t>
-  </si>
-  <si>
     <t>GUASTELLA STEFANO</t>
   </si>
   <si>
@@ -43,6 +40,18 @@
   </si>
   <si>
     <t>VESPERTINO SIMONE</t>
+  </si>
+  <si>
+    <t>GIONFRIDDO ANDREA</t>
+  </si>
+  <si>
+    <t>MANCARELLA SALVATORE</t>
+  </si>
+  <si>
+    <t>AVOLA IVAN</t>
+  </si>
+  <si>
+    <t>GOLINO KEVIN</t>
   </si>
 </sst>
 </file>
@@ -383,16 +392,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -423,7 +432,7 @@
         <v>45887</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>8</v>
@@ -434,7 +443,7 @@
         <v>45887</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
@@ -445,7 +454,7 @@
         <v>45887</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -456,7 +465,7 @@
         <v>45887</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>11</v>
@@ -467,9 +476,42 @@
         <v>45887</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
+        <v>45887</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
+        <v>45887</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2">
+        <v>45887</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
         <v>15</v>
       </c>
     </row>

</xml_diff>